<commit_message>
atualizacao oficail da bronze e da prata
</commit_message>
<xml_diff>
--- a/catálogo api.xlsx
+++ b/catálogo api.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan.dias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\trabalho_final_dados_em_transito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75368930-2C34-4E9B-89E0-43B1F0BF19A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09D7604-F4A3-40C7-AD6E-2F1DCE0984AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D2BF9542-D41A-48D8-BC33-8D7BCEDD7CC0}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D2BF9542-D41A-48D8-BC33-8D7BCEDD7CC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Parâmetros" sheetId="3" r:id="rId1"/>
     <sheet name="Objetos de retorno" sheetId="10" r:id="rId2"/>
+    <sheet name="testes" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Objetos de retorno'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">testes!$A$1:$G$127</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="189">
   <si>
     <r>
       <t>[int]</t>
@@ -1050,9 +1052,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>letreiro_completo</t>
-  </si>
-  <si>
     <t>linhas_localizadas</t>
   </si>
   <si>
@@ -1151,6 +1150,9 @@
   <si>
     <t>Amostra 
 tratada?</t>
+  </si>
+  <si>
+    <t>letreiro_completo_linha</t>
   </si>
 </sst>
 </file>
@@ -1670,25 +1672,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C722B33A-C11D-4F28-8321-D137E15A943D}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="76.140625" customWidth="1"/>
-    <col min="5" max="5" width="62.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="88.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="76.125" customWidth="1"/>
+    <col min="5" max="5" width="62.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="7" max="7" width="88.625" customWidth="1"/>
+    <col min="8" max="8" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30">
       <c r="A1" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>14</v>
@@ -1727,7 +1729,7 @@
         <v>130</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>19</v>
@@ -1742,7 +1744,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51.75">
+    <row r="3" spans="1:9" ht="39">
       <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
         <v>26</v>
@@ -1754,7 +1756,7 @@
         <v>131</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>19</v>
@@ -1769,7 +1771,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51.75">
+    <row r="4" spans="1:9" ht="42.75">
       <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
         <v>26</v>
@@ -1781,7 +1783,7 @@
         <v>131</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>22</v>
@@ -1796,7 +1798,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39">
+    <row r="5" spans="1:9" ht="28.5">
       <c r="A5" s="18"/>
       <c r="B5" s="12" t="s">
         <v>25</v>
@@ -1808,7 +1810,7 @@
         <v>132</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>19</v>
@@ -1837,7 +1839,7 @@
         <v>133</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>39</v>
@@ -1864,7 +1866,7 @@
         <v>134</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>58</v>
@@ -1875,7 +1877,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="18"/>
       <c r="B8" s="12" t="s">
         <v>60</v>
@@ -1896,7 +1898,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="18"/>
       <c r="B9" s="12" t="s">
         <v>66</v>
@@ -2009,7 +2011,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" ht="42.75">
+    <row r="14" spans="1:9" ht="28.5">
       <c r="A14" s="18"/>
       <c r="B14" s="12" t="s">
         <v>107</v>
@@ -2080,7 +2082,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:9" ht="42.75">
+    <row r="17" spans="1:9" ht="28.5">
       <c r="A17" s="18"/>
       <c r="B17" s="12" t="s">
         <v>107</v>
@@ -2112,21 +2114,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204C65E5-1210-4640-98D6-9E22F6C36C17}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="81.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="81.875" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
@@ -2219,7 +2223,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42.75">
+    <row r="5" spans="1:7" ht="28.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42.75">
+    <row r="12" spans="1:7" ht="28.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2435,7 +2439,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.5">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2459,7 +2463,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.5">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>np</v>
       </c>
       <c r="G17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2552,7 +2556,7 @@
         <v>ed</v>
       </c>
       <c r="G18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2576,7 +2580,7 @@
         <v>py</v>
       </c>
       <c r="G19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2600,7 +2604,7 @@
         <v>px</v>
       </c>
       <c r="G20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2620,7 +2624,7 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G21" t="s">
         <v>44</v>
@@ -2647,7 +2651,7 @@
         <v>np</v>
       </c>
       <c r="G22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2671,7 +2675,7 @@
         <v>ed</v>
       </c>
       <c r="G23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2695,7 +2699,7 @@
         <v>py</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2719,7 +2723,7 @@
         <v>px</v>
       </c>
       <c r="G25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2767,7 +2771,7 @@
         <v>np</v>
       </c>
       <c r="G27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2791,7 +2795,7 @@
         <v>ed</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2815,7 +2819,7 @@
         <v>py</v>
       </c>
       <c r="G29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2839,7 +2843,7 @@
         <v>px</v>
       </c>
       <c r="G30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="28.5">
@@ -2863,7 +2867,7 @@
         <v>cc</v>
       </c>
       <c r="G31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2887,7 +2891,7 @@
         <v>nc</v>
       </c>
       <c r="G32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2931,10 +2935,10 @@
         <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2957,7 +2961,7 @@
         <v>116</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2977,10 +2981,10 @@
         <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3003,7 +3007,7 @@
         <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3026,7 +3030,7 @@
         <v>154</v>
       </c>
       <c r="G38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3046,10 +3050,10 @@
         <v>78</v>
       </c>
       <c r="F39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3096,7 +3100,7 @@
         <v>143</v>
       </c>
       <c r="G41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3119,7 +3123,7 @@
         <v>154</v>
       </c>
       <c r="G42" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3145,7 +3149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30">
+    <row r="44" spans="1:7" ht="29.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3189,7 +3193,7 @@
         <v>145</v>
       </c>
       <c r="G45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3212,7 +3216,7 @@
         <v>146</v>
       </c>
       <c r="G46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3235,7 +3239,7 @@
         <v>147</v>
       </c>
       <c r="G47" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3258,7 +3262,7 @@
         <v>148</v>
       </c>
       <c r="G48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3281,7 +3285,7 @@
         <v>149</v>
       </c>
       <c r="G49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3304,7 +3308,7 @@
         <v>116</v>
       </c>
       <c r="G50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="28.5">
@@ -3327,7 +3331,7 @@
         <v>150</v>
       </c>
       <c r="G51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3350,7 +3354,7 @@
         <v>151</v>
       </c>
       <c r="G52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3373,7 +3377,7 @@
         <v>152</v>
       </c>
       <c r="G53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3420,7 +3424,7 @@
         <v>vs</v>
       </c>
       <c r="G55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3443,7 +3447,7 @@
         <v>149</v>
       </c>
       <c r="G56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3466,7 +3470,7 @@
         <v>116</v>
       </c>
       <c r="G57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="28.5">
@@ -3490,7 +3494,7 @@
         <v>ta</v>
       </c>
       <c r="G58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3514,7 +3518,7 @@
         <v>py</v>
       </c>
       <c r="G59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3538,7 +3542,7 @@
         <v>px</v>
       </c>
       <c r="G60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3585,7 +3589,7 @@
         <v>143</v>
       </c>
       <c r="G62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3608,7 +3612,7 @@
         <v>154</v>
       </c>
       <c r="G63" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -3635,7 +3639,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30">
+    <row r="65" spans="1:7" ht="29.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3679,7 +3683,7 @@
         <v>145</v>
       </c>
       <c r="G66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3702,7 +3706,7 @@
         <v>146</v>
       </c>
       <c r="G67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3725,7 +3729,7 @@
         <v>147</v>
       </c>
       <c r="G68" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3748,7 +3752,7 @@
         <v>148</v>
       </c>
       <c r="G69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3771,7 +3775,7 @@
         <v>149</v>
       </c>
       <c r="G70" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3794,7 +3798,7 @@
         <v>116</v>
       </c>
       <c r="G71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="28.5">
@@ -3817,7 +3821,7 @@
         <v>150</v>
       </c>
       <c r="G72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3841,7 +3845,7 @@
         <v>py</v>
       </c>
       <c r="G73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3865,7 +3869,7 @@
         <v>px</v>
       </c>
       <c r="G74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3912,7 +3916,7 @@
         <v>149</v>
       </c>
       <c r="G76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3960,7 +3964,7 @@
         <v>np</v>
       </c>
       <c r="G78" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3984,7 +3988,7 @@
         <v>py</v>
       </c>
       <c r="G79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -4008,7 +4012,7 @@
         <v>px</v>
       </c>
       <c r="G80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -4031,7 +4035,7 @@
         <v>143</v>
       </c>
       <c r="G81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4054,7 +4058,7 @@
         <v>154</v>
       </c>
       <c r="G82" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4081,7 +4085,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30">
+    <row r="84" spans="1:7" ht="29.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4125,7 +4129,7 @@
         <v>145</v>
       </c>
       <c r="G85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4148,7 +4152,7 @@
         <v>146</v>
       </c>
       <c r="G86" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4172,7 +4176,7 @@
         <v>qv</v>
       </c>
       <c r="G87" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4196,7 +4200,7 @@
         <v>vs</v>
       </c>
       <c r="G88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4219,7 +4223,7 @@
         <v>149</v>
       </c>
       <c r="G89" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4239,10 +4243,10 @@
         <v>115</v>
       </c>
       <c r="F90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4265,7 +4269,7 @@
         <v>116</v>
       </c>
       <c r="G91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="28.5">
@@ -4288,7 +4292,7 @@
         <v>150</v>
       </c>
       <c r="G92" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4311,7 +4315,7 @@
         <v>151</v>
       </c>
       <c r="G93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4334,10 +4338,10 @@
         <v>152</v>
       </c>
       <c r="G94" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4360,7 +4364,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" ht="15">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4377,13 +4381,13 @@
         <v>125</v>
       </c>
       <c r="F96" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G96" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4400,13 +4404,13 @@
         <v>112</v>
       </c>
       <c r="F97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G97" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" ht="15">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4427,10 +4431,10 @@
         <v>np</v>
       </c>
       <c r="G98" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4451,10 +4455,10 @@
         <v>py</v>
       </c>
       <c r="G99" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4475,10 +4479,10 @@
         <v>px</v>
       </c>
       <c r="G100" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4499,10 +4503,10 @@
         <v>vs</v>
       </c>
       <c r="G101" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4522,10 +4526,10 @@
         <v>149</v>
       </c>
       <c r="G102" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4542,13 +4546,13 @@
         <v>115</v>
       </c>
       <c r="F103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G103" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>116</v>
       </c>
       <c r="G104" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="28.5">
@@ -4591,10 +4595,10 @@
         <v>150</v>
       </c>
       <c r="G105" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4615,10 +4619,10 @@
         <v>py</v>
       </c>
       <c r="G106" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4639,10 +4643,10 @@
         <v>px</v>
       </c>
       <c r="G107" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4666,7 +4670,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" ht="15">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4686,10 +4690,10 @@
         <v>149</v>
       </c>
       <c r="G109" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4713,7 +4717,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" ht="15">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4734,10 +4738,10 @@
         <v>np</v>
       </c>
       <c r="G111" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4758,10 +4762,10 @@
         <v>py</v>
       </c>
       <c r="G112" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4782,10 +4786,10 @@
         <v>px</v>
       </c>
       <c r="G113" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4805,10 +4809,10 @@
         <v>143</v>
       </c>
       <c r="G114" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4828,10 +4832,10 @@
         <v>154</v>
       </c>
       <c r="G115" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4855,7 +4859,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="30">
+    <row r="117" spans="1:7" ht="29.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4879,7 +4883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" ht="15">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4899,10 +4903,10 @@
         <v>145</v>
       </c>
       <c r="G118" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4922,10 +4926,10 @@
         <v>146</v>
       </c>
       <c r="G119" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4946,10 +4950,10 @@
         <v>qv</v>
       </c>
       <c r="G120" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4970,10 +4974,10 @@
         <v>vs</v>
       </c>
       <c r="G121" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4993,10 +4997,10 @@
         <v>149</v>
       </c>
       <c r="G122" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5013,13 +5017,13 @@
         <v>115</v>
       </c>
       <c r="F123" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G123" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5039,7 +5043,7 @@
         <v>116</v>
       </c>
       <c r="G124" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="28.5">
@@ -5062,10 +5066,10 @@
         <v>150</v>
       </c>
       <c r="G125" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5086,10 +5090,10 @@
         <v>py</v>
       </c>
       <c r="G126" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5110,38 +5114,3078 @@
         <v>px</v>
       </c>
       <c r="G127" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" ht="15.75" thickBot="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15" thickBot="1">
       <c r="D128" s="7"/>
     </row>
     <row r="130" spans="4:4">
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="4:4" ht="15.75" thickBot="1">
+    <row r="131" spans="4:4" ht="15" thickBot="1">
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="4:4" ht="15.75" thickBot="1">
+    <row r="132" spans="4:4" ht="15" thickBot="1">
       <c r="D132" s="6"/>
     </row>
-    <row r="134" spans="4:4" ht="15.75" thickBot="1">
+    <row r="134" spans="4:4" ht="15" thickBot="1">
       <c r="D134" s="7"/>
     </row>
     <row r="136" spans="4:4">
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="4:4" ht="15.75" thickBot="1">
+    <row r="137" spans="4:4" ht="15" thickBot="1">
       <c r="D137" s="6"/>
     </row>
-    <row r="138" spans="4:4" ht="15.75" thickBot="1">
+    <row r="138" spans="4:4" ht="15" thickBot="1">
       <c r="D138" s="6"/>
     </row>
-    <row r="140" spans="4:4" ht="15.75" thickBot="1">
+    <row r="140" spans="4:4" ht="15" thickBot="1">
       <c r="D140" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{204C65E5-1210-4640-98D6-9E22F6C36C17}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C70451-B5BC-4E8B-8DB5-4D7C4EACBFD6}">
+  <dimension ref="A1:G140"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="81.875" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F20" si="0">RIGHT(D2,2)</f>
+        <v>cl</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>lc</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>lt</v>
+      </c>
+      <c r="G4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>tl</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>sl</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>tp</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>ts</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>cl</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>lc</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>lt</v>
+      </c>
+      <c r="G11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>tl</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>sl</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>tp</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>ts</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>cp</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>np</v>
+      </c>
+      <c r="G17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>ed</v>
+      </c>
+      <c r="G18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>py</v>
+      </c>
+      <c r="G19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>px</v>
+      </c>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>159</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" ref="F22:F33" si="1">RIGHT(D22,2)</f>
+        <v>np</v>
+      </c>
+      <c r="G22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>ed</v>
+      </c>
+      <c r="G23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>py</v>
+      </c>
+      <c r="G24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>px</v>
+      </c>
+      <c r="G25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v>cp</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>np</v>
+      </c>
+      <c r="G27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v>ed</v>
+      </c>
+      <c r="G28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v>py</v>
+      </c>
+      <c r="G29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v>px</v>
+      </c>
+      <c r="G30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.5">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v>cc</v>
+      </c>
+      <c r="G31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v>nc</v>
+      </c>
+      <c r="G32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v>hr</v>
+      </c>
+      <c r="G33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" t="str">
+        <f>RIGHT(D40,2)</f>
+        <v>hr</v>
+      </c>
+      <c r="G40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="29.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" t="str">
+        <f>RIGHT(D44,2)</f>
+        <v>sl</v>
+      </c>
+      <c r="G44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" t="s">
+        <v>146</v>
+      </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" t="s">
+        <v>148</v>
+      </c>
+      <c r="G48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" t="s">
+        <v>116</v>
+      </c>
+      <c r="G50" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.5">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" t="s">
+        <v>150</v>
+      </c>
+      <c r="G51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F52" t="s">
+        <v>151</v>
+      </c>
+      <c r="G52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F55" t="str">
+        <f>RIGHT(D55,2)</f>
+        <v>vs</v>
+      </c>
+      <c r="G55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.5">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" t="str">
+        <f>RIGHT(D58,2)</f>
+        <v>ta</v>
+      </c>
+      <c r="G58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F59" t="str">
+        <f>RIGHT(D59,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F60" t="str">
+        <f>RIGHT(D60,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F61" t="str">
+        <f>RIGHT(D61,2)</f>
+        <v>hr</v>
+      </c>
+      <c r="G61" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" t="s">
+        <v>143</v>
+      </c>
+      <c r="G62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" t="s">
+        <v>154</v>
+      </c>
+      <c r="G63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F64" t="str">
+        <f>RIGHT(D64,2)</f>
+        <v>cl</v>
+      </c>
+      <c r="G64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="29.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F65" t="str">
+        <f>RIGHT(D65,2)</f>
+        <v>sl</v>
+      </c>
+      <c r="G65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" t="s">
+        <v>145</v>
+      </c>
+      <c r="G66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" t="s">
+        <v>103</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F67" t="s">
+        <v>146</v>
+      </c>
+      <c r="G67" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F68" t="s">
+        <v>147</v>
+      </c>
+      <c r="G68" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" t="s">
+        <v>103</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F69" t="s">
+        <v>148</v>
+      </c>
+      <c r="G69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" t="s">
+        <v>149</v>
+      </c>
+      <c r="G70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F71" t="s">
+        <v>116</v>
+      </c>
+      <c r="G71" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="28.5">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+      <c r="G72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F73" t="str">
+        <f>RIGHT(D73,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" t="s">
+        <v>103</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F74" t="str">
+        <f>RIGHT(D74,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G74" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F75" t="str">
+        <f>RIGHT(D75,2)</f>
+        <v>hr</v>
+      </c>
+      <c r="G75" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F76" t="s">
+        <v>149</v>
+      </c>
+      <c r="G76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F77" t="str">
+        <f>RIGHT(D77,2)</f>
+        <v>cp</v>
+      </c>
+      <c r="G77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F78" t="str">
+        <f>RIGHT(D78,2)</f>
+        <v>np</v>
+      </c>
+      <c r="G78" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F79" t="str">
+        <f>RIGHT(D79,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G79" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F80" t="str">
+        <f>RIGHT(D80,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G80" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F81" t="s">
+        <v>143</v>
+      </c>
+      <c r="G81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F82" t="s">
+        <v>154</v>
+      </c>
+      <c r="G82" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F83" t="str">
+        <f>RIGHT(D83,2)</f>
+        <v>cl</v>
+      </c>
+      <c r="G83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="29.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F84" t="str">
+        <f>RIGHT(D84,2)</f>
+        <v>sl</v>
+      </c>
+      <c r="G84" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F85" t="s">
+        <v>145</v>
+      </c>
+      <c r="G85" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F86" t="s">
+        <v>146</v>
+      </c>
+      <c r="G86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>107</v>
+      </c>
+      <c r="C87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F87" t="str">
+        <f>RIGHT(D87,2)</f>
+        <v>qv</v>
+      </c>
+      <c r="G87" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" t="s">
+        <v>107</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F88" t="str">
+        <f>RIGHT(D88,2)</f>
+        <v>vs</v>
+      </c>
+      <c r="G88" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" t="s">
+        <v>149</v>
+      </c>
+      <c r="G89" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" t="s">
+        <v>107</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" t="s">
+        <v>158</v>
+      </c>
+      <c r="G90" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" t="s">
+        <v>107</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F91" t="s">
+        <v>116</v>
+      </c>
+      <c r="G91" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="28.5">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F92" t="s">
+        <v>150</v>
+      </c>
+      <c r="G92" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" t="s">
+        <v>107</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F93" t="s">
+        <v>151</v>
+      </c>
+      <c r="G93" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F94" t="s">
+        <v>152</v>
+      </c>
+      <c r="G94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F95" t="s">
+        <v>153</v>
+      </c>
+      <c r="G95" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F96" t="s">
+        <v>160</v>
+      </c>
+      <c r="G96" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" t="s">
+        <v>159</v>
+      </c>
+      <c r="G97" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F98" t="str">
+        <f>RIGHT(D98,2)</f>
+        <v>np</v>
+      </c>
+      <c r="G98" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F99" t="str">
+        <f>RIGHT(D99,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G99" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F100" t="str">
+        <f>RIGHT(D100,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G100" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F101" t="str">
+        <f>RIGHT(D101,2)</f>
+        <v>vs</v>
+      </c>
+      <c r="G101" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F102" t="s">
+        <v>149</v>
+      </c>
+      <c r="G102" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F103" t="s">
+        <v>158</v>
+      </c>
+      <c r="G103" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F104" t="s">
+        <v>116</v>
+      </c>
+      <c r="G104" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="28.5">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F105" t="s">
+        <v>150</v>
+      </c>
+      <c r="G105" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F106" t="str">
+        <f>RIGHT(D106,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G106" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F107" t="str">
+        <f>RIGHT(D107,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G107" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F108" t="str">
+        <f>RIGHT(D108,2)</f>
+        <v>hr</v>
+      </c>
+      <c r="G108" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F109" t="s">
+        <v>149</v>
+      </c>
+      <c r="G109" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F110" t="str">
+        <f>RIGHT(D110,2)</f>
+        <v>cp</v>
+      </c>
+      <c r="G110" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F111" t="str">
+        <f>RIGHT(D111,2)</f>
+        <v>np</v>
+      </c>
+      <c r="G111" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F112" t="str">
+        <f>RIGHT(D112,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G112" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F113" t="str">
+        <f>RIGHT(D113,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F114" t="s">
+        <v>143</v>
+      </c>
+      <c r="G114" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F115" t="s">
+        <v>154</v>
+      </c>
+      <c r="G115" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F116" t="str">
+        <f>RIGHT(D116,2)</f>
+        <v>cl</v>
+      </c>
+      <c r="G116" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="29.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F117" t="str">
+        <f>RIGHT(D117,2)</f>
+        <v>sl</v>
+      </c>
+      <c r="G117" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F118" t="s">
+        <v>145</v>
+      </c>
+      <c r="G118" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F119" t="s">
+        <v>146</v>
+      </c>
+      <c r="G119" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F120" t="str">
+        <f>RIGHT(D120,2)</f>
+        <v>qv</v>
+      </c>
+      <c r="G120" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F121" t="str">
+        <f>RIGHT(D121,2)</f>
+        <v>vs</v>
+      </c>
+      <c r="G121" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F122" t="s">
+        <v>149</v>
+      </c>
+      <c r="G122" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F123" t="s">
+        <v>158</v>
+      </c>
+      <c r="G123" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F124" t="s">
+        <v>116</v>
+      </c>
+      <c r="G124" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="28.5">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F125" t="s">
+        <v>150</v>
+      </c>
+      <c r="G125" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F126" t="str">
+        <f>RIGHT(D126,2)</f>
+        <v>py</v>
+      </c>
+      <c r="G126" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C127" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F127" t="str">
+        <f>RIGHT(D127,2)</f>
+        <v>px</v>
+      </c>
+      <c r="G127" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15" thickBot="1">
+      <c r="D128" s="7"/>
+    </row>
+    <row r="130" spans="4:4">
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="4:4" ht="15" thickBot="1">
+      <c r="D131" s="6"/>
+    </row>
+    <row r="132" spans="4:4" ht="15" thickBot="1">
+      <c r="D132" s="6"/>
+    </row>
+    <row r="134" spans="4:4" ht="15" thickBot="1">
+      <c r="D134" s="7"/>
+    </row>
+    <row r="136" spans="4:4">
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="4:4" ht="15" thickBot="1">
+      <c r="D137" s="6"/>
+    </row>
+    <row r="138" spans="4:4" ht="15" thickBot="1">
+      <c r="D138" s="6"/>
+    </row>
+    <row r="140" spans="4:4" ht="15" thickBot="1">
+      <c r="D140" s="7"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G127" xr:uid="{F5C70451-B5BC-4E8B-8DB5-4D7C4EACBFD6}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>